<commit_message>
making progress, stuck on edge cases pretty hard
</commit_message>
<xml_diff>
--- a/0 template/Whiteboards/Solution.xlsx
+++ b/0 template/Whiteboards/Solution.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF5CC23-22FA-4D9F-82CC-E48954E21ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BADD94D-1057-4796-B587-292548BDD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,6 +57,56 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>xpect</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>&gt;&gt;</t>
+  </si>
+  <si>
+    <t>steps</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>threads</t>
+  </si>
+  <si>
+    <t>thread</t>
+  </si>
+  <si>
+    <t>ind</t>
+  </si>
+  <si>
+    <t>}}</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -67,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,6 +167,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -144,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +233,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="F4:BA80"/>
+  <dimension ref="E4:AZ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="AL38" sqref="AL38"/>
+    <sheetView tabSelected="1" topLeftCell="O48" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AF57" sqref="AF57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1595,6 +1657,10 @@
         <f>X$26-$S29</f>
         <v>3</v>
       </c>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="3"/>
+      <c r="AO29" s="5"/>
     </row>
     <row r="30" spans="7:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S30" s="1">
@@ -1615,761 +1681,1470 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S33" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S34" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AA38" s="1">
+    <row r="40" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G40" s="1">
         <v>20</v>
       </c>
-      <c r="AB38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC38" s="1">
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1">
         <v>15</v>
       </c>
-      <c r="AD38" s="1">
+      <c r="J40" s="1">
         <v>3</v>
       </c>
-      <c r="AE38" s="1">
+      <c r="K40" s="1">
         <v>10</v>
       </c>
-      <c r="AF38" s="1">
+      <c r="L40" s="1">
         <v>5</v>
       </c>
-      <c r="AG38" s="1">
+      <c r="M40" s="1">
         <v>8</v>
       </c>
-      <c r="AJ38" s="1">
+      <c r="P40" s="1">
         <v>83</v>
       </c>
-      <c r="AK38" s="1">
+      <c r="Q40" s="1">
         <v>20</v>
       </c>
-      <c r="AL38" s="3">
+      <c r="R40" s="3">
         <v>17</v>
       </c>
-      <c r="AM38" s="5">
+      <c r="S40" s="5">
         <v>43</v>
       </c>
-      <c r="AN38" s="3">
+      <c r="T40" s="3">
         <v>52</v>
       </c>
-      <c r="AO38" s="5">
+      <c r="U40" s="5">
         <v>78</v>
       </c>
-      <c r="AP38" s="1">
+      <c r="V40" s="1">
         <v>68</v>
       </c>
-      <c r="AQ38" s="1">
+      <c r="W40" s="1">
         <v>45</v>
       </c>
-      <c r="AT38" s="6">
+      <c r="Z40" s="6">
         <v>2</v>
       </c>
-      <c r="AU38" s="6">
-        <v>1</v>
-      </c>
-      <c r="AV38" s="6">
-        <v>13</v>
-      </c>
-      <c r="AW38" s="6">
+      <c r="AA40" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="6">
+        <v>13</v>
+      </c>
+      <c r="AC40" s="6">
         <v>3</v>
       </c>
-      <c r="AX38" s="6">
+      <c r="AD40" s="6">
         <v>2</v>
       </c>
-      <c r="AY38" s="6">
+      <c r="AE40" s="6">
         <v>2</v>
       </c>
-      <c r="AZ38" s="6">
+      <c r="AF40" s="6">
         <v>15</v>
       </c>
-      <c r="BA38" s="6">
+      <c r="AG40" s="6">
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z39" s="1">
+    <row r="41" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="1">
         <v>20</v>
       </c>
-      <c r="AB39" s="1">
+      <c r="H41" s="1">
         <v>-19</v>
       </c>
-      <c r="AC39" s="3">
+      <c r="I41" s="3">
         <v>-5</v>
       </c>
-      <c r="AD39" s="1">
+      <c r="J41" s="1">
         <v>-17</v>
       </c>
-      <c r="AE39" s="1">
+      <c r="K41" s="1">
         <v>-10</v>
       </c>
-      <c r="AF39" s="1">
+      <c r="L41" s="1">
         <v>-15</v>
       </c>
-      <c r="AG39" s="1">
+      <c r="M41" s="1">
         <v>-12</v>
       </c>
-      <c r="AI39" s="1">
+      <c r="O41" s="1">
         <v>83</v>
       </c>
-      <c r="AK39" s="1">
+      <c r="Q41" s="1">
         <v>-63</v>
       </c>
-      <c r="AL39" s="1">
+      <c r="R41" s="1">
         <v>-66</v>
       </c>
-      <c r="AM39" s="1">
+      <c r="S41" s="1">
         <v>-40</v>
       </c>
-      <c r="AN39" s="1">
+      <c r="T41" s="1">
         <v>-31</v>
       </c>
-      <c r="AO39" s="1">
+      <c r="U41" s="1">
         <v>-5</v>
       </c>
-      <c r="AP39" s="1">
+      <c r="V41" s="1">
         <v>-15</v>
       </c>
-      <c r="AQ39" s="1">
+      <c r="W41" s="1">
         <v>-38</v>
       </c>
-      <c r="AS39" s="1">
+      <c r="Y41" s="1">
         <v>2</v>
       </c>
-      <c r="AU39" s="1">
+      <c r="AA41" s="1">
         <v>-1</v>
       </c>
-      <c r="AV39" s="1">
+      <c r="AB41" s="1">
         <v>11</v>
       </c>
-      <c r="AW39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AX39" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY39" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ39" s="1">
-        <v>13</v>
-      </c>
-      <c r="BA39" s="1">
+      <c r="AC41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>13</v>
+      </c>
+      <c r="AG41" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC40" s="1">
+    <row r="42" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="I42" s="1">
         <v>14</v>
       </c>
-      <c r="AD40" s="1">
+      <c r="J42" s="1">
         <v>2</v>
       </c>
-      <c r="AE40" s="1">
+      <c r="K42" s="1">
         <v>9</v>
       </c>
-      <c r="AF40" s="1">
+      <c r="L42" s="1">
         <v>4</v>
       </c>
-      <c r="AG40" s="1">
+      <c r="M42" s="1">
         <v>7</v>
       </c>
-      <c r="AI40" s="1">
+      <c r="O42" s="1">
         <v>20</v>
       </c>
-      <c r="AL40" s="1">
+      <c r="R42" s="1">
         <v>-3</v>
       </c>
-      <c r="AM40" s="1">
+      <c r="S42" s="1">
         <v>23</v>
       </c>
-      <c r="AN40" s="1">
+      <c r="T42" s="1">
         <v>32</v>
       </c>
-      <c r="AO40" s="1">
+      <c r="U42" s="1">
         <v>58</v>
       </c>
-      <c r="AP40" s="1">
+      <c r="V42" s="1">
         <v>48</v>
       </c>
-      <c r="AQ40" s="1">
+      <c r="W42" s="1">
         <v>25</v>
       </c>
-      <c r="AS40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV40" s="7">
+      <c r="Y42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="7">
         <v>12</v>
       </c>
-      <c r="AW40" s="1">
+      <c r="AC42" s="1">
         <v>2</v>
       </c>
-      <c r="AX40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AY40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AZ40" s="1">
+      <c r="AD42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF42" s="1">
         <v>14</v>
       </c>
-      <c r="BA40" s="1">
+      <c r="AG42" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="41" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z41" s="1">
+      <c r="AO42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
         <v>15</v>
       </c>
-      <c r="AD41" s="1">
+      <c r="J43" s="1">
         <v>-12</v>
       </c>
-      <c r="AE41" s="3">
+      <c r="K43" s="3">
         <v>-5</v>
       </c>
-      <c r="AF41" s="1">
+      <c r="L43" s="1">
         <v>-10</v>
       </c>
-      <c r="AG41" s="1">
+      <c r="M43" s="1">
         <v>-7</v>
       </c>
-      <c r="AI41" s="1">
+      <c r="O43" s="1">
         <v>17</v>
       </c>
-      <c r="AM41" s="1">
-        <v>26</v>
-      </c>
-      <c r="AN41" s="7">
+      <c r="S43" s="1">
+        <v>26</v>
+      </c>
+      <c r="T43" s="7">
         <v>35</v>
       </c>
-      <c r="AO41" s="1">
+      <c r="U43" s="1">
         <v>61</v>
       </c>
-      <c r="AP41" s="1">
+      <c r="V43" s="1">
         <v>51</v>
       </c>
-      <c r="AQ41" s="1">
+      <c r="W43" s="1">
         <v>28</v>
       </c>
-      <c r="AS41" s="1">
-        <v>13</v>
-      </c>
-      <c r="AW41" s="1">
+      <c r="Y43" s="1">
+        <v>13</v>
+      </c>
+      <c r="AC43" s="1">
         <v>-10</v>
       </c>
-      <c r="AX41" s="1">
+      <c r="AD43" s="1">
         <v>-11</v>
       </c>
-      <c r="AY41" s="1">
+      <c r="AE43" s="1">
         <v>-11</v>
       </c>
-      <c r="AZ41" s="1">
+      <c r="AF43" s="1">
         <v>2</v>
       </c>
-      <c r="BA41" s="7">
+      <c r="AG43" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z42" s="1">
+      <c r="AO43" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="1">
         <v>3</v>
       </c>
-      <c r="AE42" s="1">
+      <c r="K44" s="1">
         <v>7</v>
       </c>
-      <c r="AF42" s="1">
+      <c r="L44" s="1">
         <v>2</v>
       </c>
-      <c r="AG42" s="1">
+      <c r="M44" s="1">
         <v>5</v>
       </c>
-      <c r="AI42" s="1">
+      <c r="O44" s="1">
         <v>43</v>
       </c>
-      <c r="AN42" s="1">
+      <c r="T44" s="1">
         <v>9</v>
       </c>
-      <c r="AO42" s="7">
+      <c r="U44" s="7">
         <v>35</v>
       </c>
-      <c r="AP42" s="1">
+      <c r="V44" s="1">
         <v>25</v>
       </c>
-      <c r="AQ42" s="1">
+      <c r="W44" s="1">
         <v>2</v>
       </c>
-      <c r="AS42" s="1">
+      <c r="Y44" s="1">
         <v>3</v>
       </c>
-      <c r="AX42" s="1">
+      <c r="AD44" s="1">
         <v>-1</v>
       </c>
-      <c r="AY42" s="1">
+      <c r="AE44" s="1">
         <v>-1</v>
       </c>
-      <c r="AZ42" s="7">
+      <c r="AF44" s="7">
         <v>12</v>
       </c>
-      <c r="BA42" s="1">
+      <c r="AG44" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z43" s="1">
+      <c r="AO44" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
         <v>10</v>
       </c>
-      <c r="AF43" s="3">
+      <c r="L45" s="3">
         <v>-5</v>
       </c>
-      <c r="AG43" s="1">
+      <c r="M45" s="1">
         <v>-2</v>
       </c>
-      <c r="AI43" s="1">
+      <c r="O45" s="1">
         <v>52</v>
       </c>
-      <c r="AO43" s="1">
-        <v>26</v>
-      </c>
-      <c r="AP43" s="1">
+      <c r="U45" s="1">
+        <v>26</v>
+      </c>
+      <c r="V45" s="1">
         <v>16</v>
       </c>
-      <c r="AQ43" s="1">
+      <c r="W45" s="1">
         <v>-7</v>
       </c>
-      <c r="AS43" s="1">
+      <c r="Y45" s="1">
         <v>2</v>
       </c>
-      <c r="AY43" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ43" s="1">
-        <v>13</v>
-      </c>
-      <c r="BA43" s="1">
+      <c r="AE45" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>13</v>
+      </c>
+      <c r="AG45" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="44" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z44" s="1">
+      <c r="AO45" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
         <v>5</v>
       </c>
-      <c r="AG44" s="1">
+      <c r="M46" s="1">
         <v>3</v>
       </c>
-      <c r="AI44" s="1">
+      <c r="O46" s="1">
         <v>78</v>
       </c>
-      <c r="AP44" s="1">
+      <c r="V46" s="1">
         <v>-10</v>
       </c>
-      <c r="AQ44" s="1">
+      <c r="W46" s="1">
         <v>-33</v>
       </c>
-      <c r="AS44" s="1">
+      <c r="Y46" s="1">
         <v>2</v>
       </c>
-      <c r="AZ44" s="1">
-        <v>13</v>
-      </c>
-      <c r="BA44" s="1">
+      <c r="AF46" s="1">
+        <v>13</v>
+      </c>
+      <c r="AG46" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z45" s="1">
+      <c r="AO46" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
         <v>8</v>
       </c>
-      <c r="AI45" s="1">
+      <c r="O47" s="1">
         <v>68</v>
       </c>
-      <c r="AQ45" s="1">
+      <c r="W47" s="1">
         <v>-23</v>
       </c>
-      <c r="AS45" s="1">
+      <c r="Y47" s="1">
         <v>15</v>
       </c>
-      <c r="BA45" s="1">
+      <c r="AG47" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="19:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Z46" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI46" s="1">
+      <c r="AO47" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP47" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="6:42" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="O48" s="1">
         <v>45</v>
       </c>
-      <c r="AS46" s="1">
+      <c r="Y48" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="V51" s="3">
-        <v>1</v>
-      </c>
-      <c r="W51" s="8">
+    <row r="50" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO50" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP50" s="1">
         <v>2</v>
       </c>
-      <c r="X51" s="3">
+      <c r="AQ50" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR50" s="1">
+        <v>4</v>
+      </c>
+      <c r="AS50" s="1">
+        <v>5</v>
+      </c>
+      <c r="AT50" s="1">
+        <v>6</v>
+      </c>
+      <c r="AU50" s="1">
+        <v>7</v>
+      </c>
+      <c r="AV50" s="1">
+        <v>8</v>
+      </c>
+      <c r="AW50" s="1">
+        <v>9</v>
+      </c>
+      <c r="AX50" s="1">
+        <v>10</v>
+      </c>
+      <c r="AY50" s="1">
+        <v>11</v>
+      </c>
+      <c r="AZ50" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G51" s="3">
+        <v>1</v>
+      </c>
+      <c r="H51" s="8">
+        <v>2</v>
+      </c>
+      <c r="I51" s="3">
         <v>14</v>
       </c>
-      <c r="Y51" s="8">
+      <c r="J51" s="8">
         <v>15</v>
       </c>
-      <c r="Z51" s="3">
+      <c r="K51" s="3">
         <v>27</v>
       </c>
-      <c r="AA51" s="8">
+      <c r="L51" s="8">
         <v>28</v>
       </c>
-      <c r="AB51" s="3">
+      <c r="M51" s="3">
         <v>40</v>
       </c>
-      <c r="AC51" s="8">
+      <c r="N51" s="8">
         <v>41</v>
       </c>
-      <c r="AD51" s="3">
+      <c r="O51" s="3">
         <v>53</v>
       </c>
-      <c r="AE51" s="8">
+      <c r="P51" s="8">
         <v>54</v>
       </c>
-      <c r="AF51" s="3">
+      <c r="Q51" s="3">
         <v>66</v>
       </c>
-      <c r="AG51" s="8">
+      <c r="R51" s="8">
         <v>67</v>
       </c>
-      <c r="AH51" s="3">
+      <c r="S51" s="3">
         <v>79</v>
       </c>
-    </row>
-    <row r="52" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U52" s="1">
-        <v>1</v>
-      </c>
-      <c r="W52" s="1">
-        <v>1</v>
-      </c>
-      <c r="X52" s="3">
-        <v>13</v>
-      </c>
-      <c r="Y52" s="1">
+      <c r="V51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X51" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Z52" s="1">
-        <v>26</v>
-      </c>
-      <c r="AA52" s="1">
+      <c r="AC51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN51" s="10">
+        <v>1</v>
+      </c>
+      <c r="AO51" s="7">
+        <v>1</v>
+      </c>
+      <c r="AP51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ51" s="7">
+        <v>0</v>
+      </c>
+      <c r="AR51" s="10">
+        <v>1</v>
+      </c>
+      <c r="AS51" s="7">
+        <v>0</v>
+      </c>
+      <c r="AT51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU51" s="7">
+        <v>1</v>
+      </c>
+      <c r="AV51" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW51" s="7">
+        <v>66</v>
+      </c>
+      <c r="AX51" s="10">
+        <v>66</v>
+      </c>
+      <c r="AY51" s="7">
+        <v>80</v>
+      </c>
+      <c r="AZ51" s="10">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3">
+        <v>13</v>
+      </c>
+      <c r="J52" s="1">
+        <v>14</v>
+      </c>
+      <c r="K52" s="1">
+        <v>26</v>
+      </c>
+      <c r="L52" s="1">
         <v>27</v>
       </c>
-      <c r="AB52" s="1">
+      <c r="M52" s="1">
         <v>39</v>
       </c>
-      <c r="AC52" s="1">
+      <c r="N52" s="1">
         <v>40</v>
       </c>
-      <c r="AD52" s="1">
+      <c r="O52" s="1">
         <v>52</v>
       </c>
-      <c r="AE52" s="1">
+      <c r="P52" s="1">
         <v>53</v>
       </c>
-      <c r="AF52" s="1">
+      <c r="Q52" s="1">
         <v>65</v>
       </c>
+      <c r="R52" s="1">
+        <v>66</v>
+      </c>
+      <c r="S52" s="1">
+        <v>78</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="AG52" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH52" s="1">
+        <v>13</v>
+      </c>
+      <c r="AI52" s="1">
+        <v>14</v>
+      </c>
+      <c r="AJ52" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL52" s="1" cm="1">
+        <f t="array" ref="AL52:AL64">TRANSPOSE(AN50:AZ50)</f>
+        <v>0</v>
+      </c>
+      <c r="AM52" s="1" cm="1">
+        <f t="array" ref="AM52:AM64">TRANSPOSE(AN51:AZ51)</f>
+        <v>1</v>
+      </c>
+      <c r="AN52" s="11"/>
+      <c r="AO52" s="1">
+        <f>AO$51-$AM52+AO$51</f>
+        <v>1</v>
+      </c>
+      <c r="AP52" s="1">
+        <f>AP$51-$AM52+AP$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AQ52" s="1">
+        <f>AQ$51-$AM52+AQ$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AR52" s="1">
+        <f>AR$51-$AM52+AR$51</f>
+        <v>1</v>
+      </c>
+      <c r="AS52" s="1">
+        <f>AS$51-$AM52+AS$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AT52" s="1">
+        <f>AT$51-$AM52+AT$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AU52" s="1">
+        <f>AU$51-$AM52+AU$51</f>
+        <v>1</v>
+      </c>
+      <c r="AV52" s="1">
+        <f>AV$51-$AM52+AV$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AW52" s="1">
+        <f>AW$51-$AM52+AW$51</f>
+        <v>131</v>
+      </c>
+      <c r="AX52" s="1">
+        <f>AX$51-$AM52+AX$51</f>
+        <v>131</v>
+      </c>
+      <c r="AY52" s="1">
+        <f>AY$51-$AM52+AY$51</f>
+        <v>159</v>
+      </c>
+      <c r="AZ52" s="1">
+        <f>AZ$51-$AM52+AZ$51</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="1">
+        <v>2</v>
+      </c>
+      <c r="I53" s="1">
+        <v>12</v>
+      </c>
+      <c r="J53" s="8">
+        <v>13</v>
+      </c>
+      <c r="K53" s="1">
+        <v>25</v>
+      </c>
+      <c r="L53" s="1">
+        <v>26</v>
+      </c>
+      <c r="M53" s="1">
+        <v>38</v>
+      </c>
+      <c r="N53" s="1">
+        <v>39</v>
+      </c>
+      <c r="O53" s="1">
+        <v>51</v>
+      </c>
+      <c r="P53" s="1">
+        <v>52</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>64</v>
+      </c>
+      <c r="R53" s="1">
+        <v>65</v>
+      </c>
+      <c r="S53" s="1">
+        <v>77</v>
+      </c>
+      <c r="AB53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AL53" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM53" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO53" s="11"/>
+      <c r="AP53" s="1">
+        <f>AP$51-$AM53+AP$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AQ53" s="1">
+        <f>AQ$51-$AM53+AQ$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AR53" s="1">
+        <f>AR$51-$AM53+AR$51</f>
+        <v>1</v>
+      </c>
+      <c r="AS53" s="1">
+        <f>AS$51-$AM53+AS$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AT53" s="1">
+        <f>AT$51-$AM53+AT$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AU53" s="1">
+        <f>AU$51-$AM53+AU$51</f>
+        <v>1</v>
+      </c>
+      <c r="AV53" s="1">
+        <f>AV$51-$AM53+AV$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AW53" s="1">
+        <f>AW$51-$AM53+AW$51</f>
+        <v>131</v>
+      </c>
+      <c r="AX53" s="1">
+        <f>AX$51-$AM53+AX$51</f>
+        <v>131</v>
+      </c>
+      <c r="AY53" s="1">
+        <f>AY$51-$AM53+AY$51</f>
+        <v>159</v>
+      </c>
+      <c r="AZ53" s="1">
+        <f>AZ$51-$AM53+AZ$51</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F54" s="1">
+        <v>14</v>
+      </c>
+      <c r="J54" s="1">
+        <v>1</v>
+      </c>
+      <c r="K54" s="3">
+        <v>13</v>
+      </c>
+      <c r="L54" s="1">
+        <v>14</v>
+      </c>
+      <c r="M54" s="1">
+        <v>26</v>
+      </c>
+      <c r="N54" s="1">
+        <v>27</v>
+      </c>
+      <c r="O54" s="1">
+        <v>39</v>
+      </c>
+      <c r="P54" s="1">
+        <v>40</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>52</v>
+      </c>
+      <c r="R54" s="1">
+        <v>53</v>
+      </c>
+      <c r="S54" s="1">
+        <v>65</v>
+      </c>
+      <c r="V54" s="1">
+        <v>14</v>
+      </c>
+      <c r="W54" s="1">
+        <v>0</v>
+      </c>
+      <c r="X54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="1">
+        <v>14</v>
+      </c>
+      <c r="AD54" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL54" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP54" s="11"/>
+      <c r="AQ54" s="1">
+        <f>AQ$51-$AM54+AQ$51</f>
+        <v>0</v>
+      </c>
+      <c r="AR54" s="1">
+        <f>AR$51-$AM54+AR$51</f>
+        <v>2</v>
+      </c>
+      <c r="AS54" s="1">
+        <f>AS$51-$AM54+AS$51</f>
+        <v>0</v>
+      </c>
+      <c r="AT54" s="1">
+        <f>AT$51-$AM54+AT$51</f>
+        <v>0</v>
+      </c>
+      <c r="AU54" s="1">
+        <f>AU$51-$AM54+AU$51</f>
+        <v>2</v>
+      </c>
+      <c r="AV54" s="1">
+        <f>AV$51-$AM54+AV$51</f>
+        <v>0</v>
+      </c>
+      <c r="AW54" s="1">
+        <f>AW$51-$AM54+AW$51</f>
+        <v>132</v>
+      </c>
+      <c r="AX54" s="1">
+        <f>AX$51-$AM54+AX$51</f>
+        <v>132</v>
+      </c>
+      <c r="AY54" s="1">
+        <f>AY$51-$AM54+AY$51</f>
+        <v>160</v>
+      </c>
+      <c r="AZ54" s="1">
+        <f>AZ$51-$AM54+AZ$51</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F55" s="1">
+        <v>15</v>
+      </c>
+      <c r="K55" s="1">
+        <v>12</v>
+      </c>
+      <c r="L55" s="8">
+        <v>13</v>
+      </c>
+      <c r="M55" s="1">
+        <v>25</v>
+      </c>
+      <c r="N55" s="1">
+        <v>26</v>
+      </c>
+      <c r="O55" s="1">
+        <v>38</v>
+      </c>
+      <c r="P55" s="1">
+        <v>39</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>51</v>
+      </c>
+      <c r="R55" s="1">
+        <v>52</v>
+      </c>
+      <c r="S55" s="1">
+        <v>64</v>
+      </c>
+      <c r="V55" s="1">
+        <v>53</v>
+      </c>
+      <c r="W55" s="1">
+        <v>13</v>
+      </c>
+      <c r="X55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC55" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD55" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL55" s="1">
+        <v>3</v>
+      </c>
+      <c r="AM55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ55" s="11"/>
+      <c r="AR55" s="1">
+        <f>AR$51-$AM55+AR$51</f>
+        <v>2</v>
+      </c>
+      <c r="AS55" s="1">
+        <f>AS$51-$AM55+AS$51</f>
+        <v>0</v>
+      </c>
+      <c r="AT55" s="1">
+        <f>AT$51-$AM55+AT$51</f>
+        <v>0</v>
+      </c>
+      <c r="AU55" s="1">
+        <f>AU$51-$AM55+AU$51</f>
+        <v>2</v>
+      </c>
+      <c r="AV55" s="1">
+        <f>AV$51-$AM55+AV$51</f>
+        <v>0</v>
+      </c>
+      <c r="AW55" s="1">
+        <f>AW$51-$AM55+AW$51</f>
+        <v>132</v>
+      </c>
+      <c r="AX55" s="1">
+        <f>AX$51-$AM55+AX$51</f>
+        <v>132</v>
+      </c>
+      <c r="AY55" s="1">
+        <f>AY$51-$AM55+AY$51</f>
+        <v>160</v>
+      </c>
+      <c r="AZ55" s="1">
+        <f>AZ$51-$AM55+AZ$51</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F56" s="1">
+        <v>27</v>
+      </c>
+      <c r="L56" s="1">
+        <v>1</v>
+      </c>
+      <c r="M56" s="3">
+        <v>13</v>
+      </c>
+      <c r="N56" s="1">
+        <v>14</v>
+      </c>
+      <c r="O56" s="1">
+        <v>26</v>
+      </c>
+      <c r="P56" s="1">
+        <v>27</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>39</v>
+      </c>
+      <c r="R56" s="1">
+        <v>40</v>
+      </c>
+      <c r="S56" s="1">
+        <v>52</v>
+      </c>
+      <c r="W56" s="1">
+        <v>26</v>
+      </c>
+      <c r="X56" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB56" s="1">
+        <v>3</v>
+      </c>
+      <c r="AL56" s="1">
+        <v>4</v>
+      </c>
+      <c r="AM56" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR56" s="11"/>
+      <c r="AS56" s="1">
+        <f>AS$51-$AM56+AS$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AT56" s="1">
+        <f>AT$51-$AM56+AT$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AU56" s="1">
+        <f>AU$51-$AM56+AU$51</f>
+        <v>1</v>
+      </c>
+      <c r="AV56" s="1">
+        <f>AV$51-$AM56+AV$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AW56" s="1">
+        <f>AW$51-$AM56+AW$51</f>
+        <v>131</v>
+      </c>
+      <c r="AX56" s="1">
+        <f>AX$51-$AM56+AX$51</f>
+        <v>131</v>
+      </c>
+      <c r="AY56" s="1">
+        <f>AY$51-$AM56+AY$51</f>
+        <v>159</v>
+      </c>
+      <c r="AZ56" s="1">
+        <f>AZ$51-$AM56+AZ$51</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F57" s="1">
+        <v>28</v>
+      </c>
+      <c r="M57" s="1">
+        <v>12</v>
+      </c>
+      <c r="N57" s="8">
+        <v>13</v>
+      </c>
+      <c r="O57" s="1">
+        <v>25</v>
+      </c>
+      <c r="P57" s="1">
+        <v>26</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>38</v>
+      </c>
+      <c r="R57" s="1">
+        <v>39</v>
+      </c>
+      <c r="S57" s="1">
+        <v>51</v>
+      </c>
+      <c r="AB57" s="1">
+        <v>4</v>
+      </c>
+      <c r="AL57" s="1">
+        <v>5</v>
+      </c>
+      <c r="AM57" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="11"/>
+      <c r="AT57" s="1">
+        <f>AT$51-$AM57+AT$51</f>
+        <v>0</v>
+      </c>
+      <c r="AU57" s="1">
+        <f>AU$51-$AM57+AU$51</f>
+        <v>2</v>
+      </c>
+      <c r="AV57" s="1">
+        <f>AV$51-$AM57+AV$51</f>
+        <v>0</v>
+      </c>
+      <c r="AW57" s="1">
+        <f>AW$51-$AM57+AW$51</f>
+        <v>132</v>
+      </c>
+      <c r="AX57" s="1">
+        <f>AX$51-$AM57+AX$51</f>
+        <v>132</v>
+      </c>
+      <c r="AY57" s="1">
+        <f>AY$51-$AM57+AY$51</f>
+        <v>160</v>
+      </c>
+      <c r="AZ57" s="1">
+        <f>AZ$51-$AM57+AZ$51</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F58" s="1">
+        <v>40</v>
+      </c>
+      <c r="N58" s="1">
+        <v>1</v>
+      </c>
+      <c r="O58" s="3">
+        <v>13</v>
+      </c>
+      <c r="P58" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>26</v>
+      </c>
+      <c r="R58" s="1">
+        <v>27</v>
+      </c>
+      <c r="S58" s="1">
+        <v>39</v>
+      </c>
+      <c r="AL58" s="1">
+        <v>6</v>
+      </c>
+      <c r="AM58" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT58" s="11"/>
+      <c r="AU58" s="1">
+        <f>AU$51-$AM58+AU$51</f>
+        <v>2</v>
+      </c>
+      <c r="AV58" s="1">
+        <f>AV$51-$AM58+AV$51</f>
+        <v>0</v>
+      </c>
+      <c r="AW58" s="1">
+        <f>AW$51-$AM58+AW$51</f>
+        <v>132</v>
+      </c>
+      <c r="AX58" s="1">
+        <f>AX$51-$AM58+AX$51</f>
+        <v>132</v>
+      </c>
+      <c r="AY58" s="1">
+        <f>AY$51-$AM58+AY$51</f>
+        <v>160</v>
+      </c>
+      <c r="AZ58" s="1">
+        <f>AZ$51-$AM58+AZ$51</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F59" s="1">
+        <v>41</v>
+      </c>
+      <c r="O59" s="1">
+        <v>12</v>
+      </c>
+      <c r="P59" s="8">
+        <v>13</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>25</v>
+      </c>
+      <c r="R59" s="1">
+        <v>26</v>
+      </c>
+      <c r="S59" s="1">
+        <v>38</v>
+      </c>
+      <c r="AL59" s="1">
+        <v>7</v>
+      </c>
+      <c r="AM59" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU59" s="11"/>
+      <c r="AV59" s="1">
+        <f>AV$51-$AM59+AV$51</f>
+        <v>-1</v>
+      </c>
+      <c r="AW59" s="1">
+        <f>AW$51-$AM59+AW$51</f>
+        <v>131</v>
+      </c>
+      <c r="AX59" s="1">
+        <f>AX$51-$AM59+AX$51</f>
+        <v>131</v>
+      </c>
+      <c r="AY59" s="1">
+        <f>AY$51-$AM59+AY$51</f>
+        <v>159</v>
+      </c>
+      <c r="AZ59" s="1">
+        <f>AZ$51-$AM59+AZ$51</f>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F60" s="1">
+        <v>53</v>
+      </c>
+      <c r="P60" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>13</v>
+      </c>
+      <c r="R60" s="1">
+        <v>14</v>
+      </c>
+      <c r="S60" s="1">
+        <v>26</v>
+      </c>
+      <c r="AD60" s="1">
+        <v>27</v>
+      </c>
+      <c r="AE60" s="1">
+        <v>13</v>
+      </c>
+      <c r="AL60" s="1">
+        <v>8</v>
+      </c>
+      <c r="AM60" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV60" s="11"/>
+      <c r="AW60" s="1">
+        <f>AW$51-$AM60+AW$51</f>
+        <v>132</v>
+      </c>
+      <c r="AX60" s="1">
+        <f>AX$51-$AM60+AX$51</f>
+        <v>132</v>
+      </c>
+      <c r="AY60" s="1">
+        <f>AY$51-$AM60+AY$51</f>
+        <v>160</v>
+      </c>
+      <c r="AZ60" s="1">
+        <f>AZ$51-$AM60+AZ$51</f>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="61" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="1">
+        <v>54</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>12</v>
+      </c>
+      <c r="R61" s="8">
+        <v>13</v>
+      </c>
+      <c r="S61" s="1">
+        <v>25</v>
+      </c>
+      <c r="AL61" s="1">
+        <v>9</v>
+      </c>
+      <c r="AM61" s="1">
         <v>66</v>
       </c>
-      <c r="AH52" s="1">
+      <c r="AW61" s="11"/>
+      <c r="AX61" s="1">
+        <f>AX$51-$AM61+AX$51</f>
+        <v>66</v>
+      </c>
+      <c r="AY61" s="1">
+        <f>AY$51-$AM61+AY$51</f>
+        <v>94</v>
+      </c>
+      <c r="AZ61" s="1">
+        <f>AZ$51-$AM61+AZ$51</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F62" s="1">
+        <v>66</v>
+      </c>
+      <c r="R62" s="1">
+        <v>1</v>
+      </c>
+      <c r="S62" s="3">
+        <v>13</v>
+      </c>
+      <c r="V62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL62" s="1">
+        <v>10</v>
+      </c>
+      <c r="AM62" s="1">
+        <v>66</v>
+      </c>
+      <c r="AX62" s="11"/>
+      <c r="AY62" s="1">
+        <f>AY$51-$AM62+AY$51</f>
+        <v>94</v>
+      </c>
+      <c r="AZ62" s="1">
+        <f>AZ$51-$AM62+AZ$51</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F63" s="1">
+        <v>67</v>
+      </c>
+      <c r="S63" s="1">
+        <v>12</v>
+      </c>
+      <c r="V63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL63" s="1">
+        <v>11</v>
+      </c>
+      <c r="AM63" s="1">
+        <v>80</v>
+      </c>
+      <c r="AY63" s="11"/>
+      <c r="AZ63" s="1">
+        <f>AZ$51-$AM63+AZ$51</f>
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U53" s="1">
+    <row r="64" spans="6:52" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F64" s="1">
+        <v>79</v>
+      </c>
+      <c r="AL64" s="1">
+        <v>12</v>
+      </c>
+      <c r="AM64" s="1">
+        <v>79</v>
+      </c>
+      <c r="AZ64" s="11"/>
+    </row>
+    <row r="66" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V66" s="1">
+        <v>0</v>
+      </c>
+      <c r="W66" s="1">
+        <v>1</v>
+      </c>
+      <c r="X66" s="1">
         <v>2</v>
       </c>
-      <c r="X53" s="1">
+      <c r="Y66" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z66" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA66" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB66" s="1">
+        <v>6</v>
+      </c>
+      <c r="AC66" s="1">
+        <v>7</v>
+      </c>
+      <c r="AD66" s="1">
+        <v>8</v>
+      </c>
+      <c r="AE66" s="1">
+        <v>9</v>
+      </c>
+      <c r="AF66" s="1">
+        <v>10</v>
+      </c>
+      <c r="AG66" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH66" s="1">
         <v>12</v>
       </c>
-      <c r="Y53" s="8">
-        <v>13</v>
-      </c>
-      <c r="Z53" s="1">
-        <v>25</v>
-      </c>
-      <c r="AA53" s="1">
-        <v>26</v>
-      </c>
-      <c r="AB53" s="1">
-        <v>38</v>
-      </c>
-      <c r="AC53" s="1">
-        <v>39</v>
-      </c>
-      <c r="AD53" s="1">
-        <v>51</v>
-      </c>
-      <c r="AE53" s="1">
-        <v>52</v>
-      </c>
-      <c r="AF53" s="1">
-        <v>64</v>
-      </c>
-      <c r="AG53" s="1">
-        <v>65</v>
-      </c>
-      <c r="AH53" s="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U54" s="1">
+    </row>
+    <row r="67" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="8">
+        <v>2</v>
+      </c>
+      <c r="H67" s="3">
         <v>14</v>
       </c>
-      <c r="Y54" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z54" s="3">
-        <v>13</v>
-      </c>
-      <c r="AA54" s="1">
-        <v>14</v>
-      </c>
-      <c r="AB54" s="1">
-        <v>26</v>
-      </c>
-      <c r="AC54" s="1">
+      <c r="I67" s="8">
+        <v>15</v>
+      </c>
+      <c r="J67" s="8">
+        <v>28</v>
+      </c>
+      <c r="K67" s="3">
         <v>27</v>
-      </c>
-      <c r="AD54" s="1">
-        <v>39</v>
-      </c>
-      <c r="AE54" s="1">
-        <v>40</v>
-      </c>
-      <c r="AF54" s="1">
-        <v>52</v>
-      </c>
-      <c r="AG54" s="1">
-        <v>53</v>
-      </c>
-      <c r="AH54" s="1">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U55" s="1">
-        <v>15</v>
-      </c>
-      <c r="Z55" s="1">
-        <v>12</v>
-      </c>
-      <c r="AA55" s="8">
-        <v>13</v>
-      </c>
-      <c r="AB55" s="1">
-        <v>25</v>
-      </c>
-      <c r="AC55" s="1">
-        <v>26</v>
-      </c>
-      <c r="AD55" s="1">
-        <v>38</v>
-      </c>
-      <c r="AE55" s="1">
-        <v>39</v>
-      </c>
-      <c r="AF55" s="1">
-        <v>51</v>
-      </c>
-      <c r="AG55" s="1">
-        <v>52</v>
-      </c>
-      <c r="AH55" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="56" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U56" s="1">
-        <v>27</v>
-      </c>
-      <c r="AA56" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB56" s="3">
-        <v>13</v>
-      </c>
-      <c r="AC56" s="1">
-        <v>14</v>
-      </c>
-      <c r="AD56" s="1">
-        <v>26</v>
-      </c>
-      <c r="AE56" s="1">
-        <v>27</v>
-      </c>
-      <c r="AF56" s="1">
-        <v>39</v>
-      </c>
-      <c r="AG56" s="1">
-        <v>40</v>
-      </c>
-      <c r="AH56" s="1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U57" s="1">
-        <v>28</v>
-      </c>
-      <c r="AB57" s="1">
-        <v>12</v>
-      </c>
-      <c r="AC57" s="8">
-        <v>13</v>
-      </c>
-      <c r="AD57" s="1">
-        <v>25</v>
-      </c>
-      <c r="AE57" s="1">
-        <v>26</v>
-      </c>
-      <c r="AF57" s="1">
-        <v>38</v>
-      </c>
-      <c r="AG57" s="1">
-        <v>39</v>
-      </c>
-      <c r="AH57" s="1">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U58" s="1">
-        <v>40</v>
-      </c>
-      <c r="AC58" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD58" s="3">
-        <v>13</v>
-      </c>
-      <c r="AE58" s="1">
-        <v>14</v>
-      </c>
-      <c r="AF58" s="1">
-        <v>26</v>
-      </c>
-      <c r="AG58" s="1">
-        <v>27</v>
-      </c>
-      <c r="AH58" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U59" s="1">
-        <v>41</v>
-      </c>
-      <c r="AD59" s="1">
-        <v>12</v>
-      </c>
-      <c r="AE59" s="8">
-        <v>13</v>
-      </c>
-      <c r="AF59" s="1">
-        <v>25</v>
-      </c>
-      <c r="AG59" s="1">
-        <v>26</v>
-      </c>
-      <c r="AH59" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="60" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U60" s="1">
-        <v>53</v>
-      </c>
-      <c r="AE60" s="1">
-        <v>1</v>
-      </c>
-      <c r="AF60" s="3">
-        <v>13</v>
-      </c>
-      <c r="AG60" s="1">
-        <v>14</v>
-      </c>
-      <c r="AH60" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U61" s="1">
-        <v>54</v>
-      </c>
-      <c r="AF61" s="1">
-        <v>12</v>
-      </c>
-      <c r="AG61" s="8">
-        <v>13</v>
-      </c>
-      <c r="AH61" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U62" s="1">
-        <v>66</v>
-      </c>
-      <c r="AG62" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH62" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="63" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U63" s="1">
-        <v>67</v>
-      </c>
-      <c r="AH63" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="21:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U64" s="1">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G67" s="3">
-        <v>1</v>
-      </c>
-      <c r="H67" s="8">
-        <v>2</v>
-      </c>
-      <c r="I67" s="3">
-        <v>14</v>
-      </c>
-      <c r="J67" s="8">
-        <v>15</v>
-      </c>
-      <c r="K67" s="8">
-        <v>28</v>
       </c>
       <c r="L67" s="3">
         <v>27</v>
@@ -2378,21 +3153,18 @@
         <v>27</v>
       </c>
       <c r="N67" s="3">
-        <v>27</v>
-      </c>
-      <c r="O67" s="3">
         <v>40</v>
       </c>
-      <c r="P67" s="8">
+      <c r="O67" s="8">
         <v>41</v>
       </c>
-      <c r="Q67" s="3">
+      <c r="P67" s="3">
         <v>53</v>
       </c>
-      <c r="R67" s="8">
+      <c r="Q67" s="8">
         <v>54</v>
       </c>
-      <c r="S67" s="3">
+      <c r="R67" s="3">
         <v>66</v>
       </c>
       <c r="V67" s="10">
@@ -2435,21 +3207,24 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F68" s="1">
-        <v>1</v>
-      </c>
-      <c r="H68" s="1">
-        <v>1</v>
-      </c>
-      <c r="I68" s="3">
-        <v>13</v>
+    <row r="68" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>1</v>
+      </c>
+      <c r="H68" s="3">
+        <v>13</v>
+      </c>
+      <c r="I68" s="1">
+        <v>14</v>
       </c>
       <c r="J68" s="1">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="K68" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L68" s="1">
         <v>26</v>
@@ -2458,22 +3233,23 @@
         <v>26</v>
       </c>
       <c r="N68" s="1">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O68" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P68" s="1">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="Q68" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R68" s="1">
-        <v>53</v>
-      </c>
-      <c r="S68" s="1">
         <v>65</v>
+      </c>
+      <c r="T68" s="1" cm="1">
+        <f t="array" ref="T68:T80">TRANSPOSE(V66:AH66)</f>
+        <v>0</v>
       </c>
       <c r="U68" s="1">
         <v>1</v>
@@ -2516,18 +3292,21 @@
         <v>78</v>
       </c>
     </row>
-    <row r="69" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F69" s="1">
+    <row r="69" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E69" s="1">
         <v>2</v>
       </c>
-      <c r="I69" s="1">
+      <c r="H69" s="1">
         <v>12</v>
       </c>
-      <c r="J69" s="8">
-        <v>13</v>
+      <c r="I69" s="8">
+        <v>13</v>
+      </c>
+      <c r="J69" s="1">
+        <v>26</v>
       </c>
       <c r="K69" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L69" s="1">
         <v>25</v>
@@ -2536,22 +3315,22 @@
         <v>25</v>
       </c>
       <c r="N69" s="1">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="O69" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P69" s="1">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="Q69" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R69" s="1">
-        <v>52</v>
-      </c>
-      <c r="S69" s="1">
         <v>64</v>
+      </c>
+      <c r="T69" s="1">
+        <v>1</v>
       </c>
       <c r="U69" s="1">
         <v>14</v>
@@ -2592,39 +3371,42 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F70" s="1">
+    <row r="70" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E70" s="1">
         <v>14</v>
       </c>
+      <c r="I70" s="1">
+        <v>1</v>
+      </c>
       <c r="J70" s="1">
-        <v>1</v>
-      </c>
-      <c r="K70" s="1">
         <v>14</v>
       </c>
-      <c r="L70" s="3">
+      <c r="K70" s="3">
+        <v>13</v>
+      </c>
+      <c r="L70" s="9">
         <v>13</v>
       </c>
       <c r="M70" s="9">
         <v>13</v>
       </c>
-      <c r="N70" s="9">
-        <v>13</v>
+      <c r="N70" s="1">
+        <v>26</v>
       </c>
       <c r="O70" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P70" s="1">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="Q70" s="1">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R70" s="1">
-        <v>40</v>
-      </c>
-      <c r="S70" s="1">
         <v>52</v>
+      </c>
+      <c r="T70" s="1">
+        <v>2</v>
       </c>
       <c r="U70" s="1">
         <v>14</v>
@@ -2663,12 +3445,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F71" s="1">
+    <row r="71" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="1">
         <v>15</v>
       </c>
-      <c r="K71" s="8">
-        <v>13</v>
+      <c r="J71" s="8">
+        <v>13</v>
+      </c>
+      <c r="K71" s="1">
+        <v>12</v>
       </c>
       <c r="L71" s="1">
         <v>12</v>
@@ -2677,22 +3462,22 @@
         <v>12</v>
       </c>
       <c r="N71" s="1">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="O71" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P71" s="1">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="Q71" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="R71" s="1">
-        <v>39</v>
-      </c>
-      <c r="S71" s="1">
         <v>51</v>
+      </c>
+      <c r="T71" s="1">
+        <v>3</v>
       </c>
       <c r="U71" s="1">
         <v>27</v>
@@ -2729,9 +3514,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F72" s="1">
+    <row r="72" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E72" s="1">
         <v>28</v>
+      </c>
+      <c r="K72" s="1">
+        <v>-1</v>
       </c>
       <c r="L72" s="1">
         <v>-1</v>
@@ -2740,22 +3528,22 @@
         <v>-1</v>
       </c>
       <c r="N72" s="1">
-        <v>-1</v>
-      </c>
-      <c r="O72" s="1">
         <v>12</v>
       </c>
-      <c r="P72" s="8">
-        <v>13</v>
+      <c r="O72" s="8">
+        <v>13</v>
+      </c>
+      <c r="P72" s="1">
+        <v>25</v>
       </c>
       <c r="Q72" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R72" s="1">
-        <v>26</v>
-      </c>
-      <c r="S72" s="1">
         <v>38</v>
+      </c>
+      <c r="T72" s="1">
+        <v>4</v>
       </c>
       <c r="U72" s="1">
         <v>27</v>
@@ -2790,30 +3578,33 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F73" s="1">
+    <row r="73" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E73" s="1">
         <v>27</v>
       </c>
+      <c r="L73" s="1">
+        <v>0</v>
+      </c>
       <c r="M73" s="1">
         <v>0</v>
       </c>
-      <c r="N73" s="1">
-        <v>0</v>
-      </c>
-      <c r="O73" s="9">
-        <v>13</v>
+      <c r="N73" s="9">
+        <v>13</v>
+      </c>
+      <c r="O73" s="1">
+        <v>14</v>
       </c>
       <c r="P73" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="Q73" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R73" s="1">
-        <v>27</v>
-      </c>
-      <c r="S73" s="1">
         <v>39</v>
+      </c>
+      <c r="T73" s="1">
+        <v>5</v>
       </c>
       <c r="U73" s="1">
         <v>40</v>
@@ -2846,27 +3637,30 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F74" s="1">
+    <row r="74" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E74" s="1">
         <v>27</v>
       </c>
-      <c r="N74" s="1">
-        <v>0</v>
-      </c>
-      <c r="O74" s="9">
-        <v>13</v>
+      <c r="M74" s="1">
+        <v>0</v>
+      </c>
+      <c r="N74" s="9">
+        <v>13</v>
+      </c>
+      <c r="O74" s="1">
+        <v>14</v>
       </c>
       <c r="P74" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="Q74" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R74" s="1">
-        <v>27</v>
-      </c>
-      <c r="S74" s="1">
         <v>39</v>
+      </c>
+      <c r="T74" s="1">
+        <v>6</v>
       </c>
       <c r="U74" s="1">
         <v>40</v>
@@ -2897,24 +3691,27 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F75" s="1">
+    <row r="75" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E75" s="1">
         <v>27</v>
       </c>
-      <c r="O75" s="9">
-        <v>13</v>
+      <c r="N75" s="9">
+        <v>13</v>
+      </c>
+      <c r="O75" s="1">
+        <v>14</v>
       </c>
       <c r="P75" s="1">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="Q75" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R75" s="1">
-        <v>27</v>
-      </c>
-      <c r="S75" s="1">
         <v>39</v>
+      </c>
+      <c r="T75" s="1">
+        <v>7</v>
       </c>
       <c r="U75" s="1">
         <v>53</v>
@@ -2943,21 +3740,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F76" s="1">
+    <row r="76" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E76" s="1">
         <v>40</v>
       </c>
-      <c r="P76" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q76" s="3">
-        <v>13</v>
+      <c r="O76" s="1">
+        <v>1</v>
+      </c>
+      <c r="P76" s="3">
+        <v>13</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>14</v>
       </c>
       <c r="R76" s="1">
-        <v>14</v>
-      </c>
-      <c r="S76" s="1">
-        <v>26</v>
+        <v>26</v>
+      </c>
+      <c r="T76" s="1">
+        <v>8</v>
       </c>
       <c r="U76" s="1">
         <v>53</v>
@@ -2984,18 +3784,21 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F77" s="1">
+    <row r="77" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E77" s="1">
         <v>41</v>
       </c>
-      <c r="Q77" s="1">
+      <c r="P77" s="1">
         <v>12</v>
       </c>
-      <c r="R77" s="8">
-        <v>13</v>
-      </c>
-      <c r="S77" s="1">
+      <c r="Q77" s="8">
+        <v>13</v>
+      </c>
+      <c r="R77" s="1">
         <v>25</v>
+      </c>
+      <c r="T77" s="1">
+        <v>9</v>
       </c>
       <c r="U77" s="1">
         <v>66</v>
@@ -3020,15 +3823,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F78" s="1">
+    <row r="78" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E78" s="1">
         <v>53</v>
       </c>
-      <c r="R78" s="1">
-        <v>1</v>
-      </c>
-      <c r="S78" s="3">
-        <v>13</v>
+      <c r="Q78" s="1">
+        <v>1</v>
+      </c>
+      <c r="R78" s="3">
+        <v>13</v>
+      </c>
+      <c r="T78" s="1">
+        <v>10</v>
       </c>
       <c r="U78" s="1">
         <v>66</v>
@@ -3051,12 +3857,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F79" s="1">
+    <row r="79" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E79" s="1">
         <v>54</v>
       </c>
-      <c r="S79" s="1">
+      <c r="R79" s="1">
         <v>12</v>
+      </c>
+      <c r="T79" s="1">
+        <v>11</v>
       </c>
       <c r="U79" s="1">
         <v>80</v>
@@ -3077,9 +3886,12 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="6:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F80" s="1">
+    <row r="80" spans="5:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E80" s="1">
         <v>66</v>
+      </c>
+      <c r="T80" s="1">
+        <v>12</v>
       </c>
       <c r="U80" s="1">
         <v>79</v>
@@ -3098,8 +3910,742 @@
       <c r="AG80" s="6"/>
       <c r="AH80" s="6"/>
     </row>
+    <row r="89" spans="10:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="1">
+        <v>0</v>
+      </c>
+      <c r="K89" s="1">
+        <v>1</v>
+      </c>
+      <c r="L89" s="1">
+        <v>2</v>
+      </c>
+      <c r="M89" s="1">
+        <v>3</v>
+      </c>
+      <c r="N89" s="1">
+        <v>4</v>
+      </c>
+      <c r="O89" s="1">
+        <v>5</v>
+      </c>
+      <c r="P89" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>7</v>
+      </c>
+      <c r="R89" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="10:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="1">
+        <v>24</v>
+      </c>
+      <c r="K90" s="1">
+        <v>13</v>
+      </c>
+      <c r="L90" s="1">
+        <v>1</v>
+      </c>
+      <c r="M90" s="1">
+        <v>100</v>
+      </c>
+      <c r="N90" s="1">
+        <v>0</v>
+      </c>
+      <c r="O90" s="1">
+        <v>94</v>
+      </c>
+      <c r="P90" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>0</v>
+      </c>
+      <c r="R90" s="1">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4393321F-B9A1-4303-8FDD-85824D72A2B2}">
+  <dimension ref="A1:L70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>35</v>
+      </c>
+      <c r="E19" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>27</v>
+      </c>
+      <c r="E24" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <v>31</v>
+      </c>
+      <c r="E27" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>35</v>
+      </c>
+      <c r="E32" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>35</v>
+      </c>
+      <c r="E34" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>39</v>
+      </c>
+      <c r="E35" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>-4</v>
+      </c>
+      <c r="E47">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>43</v>
+      </c>
+      <c r="D61">
+        <v>47</v>
+      </c>
+      <c r="E61" s="13">
+        <v>4</v>
+      </c>
+      <c r="G61">
+        <v>43</v>
+      </c>
+      <c r="H61">
+        <f>G61-4</f>
+        <v>39</v>
+      </c>
+      <c r="I61">
+        <f t="shared" ref="I61:L61" si="0">H61-4</f>
+        <v>35</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="K61">
+        <f>J61-4</f>
+        <v>27</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
solution workbook and random testing a while back
</commit_message>
<xml_diff>
--- a/0 template/Whiteboards/Solution.xlsx
+++ b/0 template/Whiteboards/Solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BADD94D-1057-4796-B587-292548BDD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E44EE4E-880A-42B4-BEA0-2EFC8705D3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -554,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
   <dimension ref="E4:AZ90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O48" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O47" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="AF57" sqref="AF57"/>
     </sheetView>
   </sheetViews>
@@ -2339,51 +2339,51 @@
       </c>
       <c r="AN52" s="11"/>
       <c r="AO52" s="1">
-        <f>AO$51-$AM52+AO$51</f>
+        <f t="shared" ref="AO52:AZ52" si="10">AO$51-$AM52+AO$51</f>
         <v>1</v>
       </c>
       <c r="AP52" s="1">
-        <f>AP$51-$AM52+AP$51</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="AQ52" s="1">
-        <f>AQ$51-$AM52+AQ$51</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="AR52" s="1">
-        <f>AR$51-$AM52+AR$51</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AS52" s="1">
-        <f>AS$51-$AM52+AS$51</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="AT52" s="1">
-        <f>AT$51-$AM52+AT$51</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="AU52" s="1">
-        <f>AU$51-$AM52+AU$51</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AV52" s="1">
-        <f>AV$51-$AM52+AV$51</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="AW52" s="1">
-        <f>AW$51-$AM52+AW$51</f>
+        <f t="shared" si="10"/>
         <v>131</v>
       </c>
       <c r="AX52" s="1">
-        <f>AX$51-$AM52+AX$51</f>
+        <f t="shared" si="10"/>
         <v>131</v>
       </c>
       <c r="AY52" s="1">
-        <f>AY$51-$AM52+AY$51</f>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="AZ52" s="1">
-        <f>AZ$51-$AM52+AZ$51</f>
+        <f t="shared" si="10"/>
         <v>157</v>
       </c>
     </row>
@@ -2441,47 +2441,47 @@
       </c>
       <c r="AO53" s="11"/>
       <c r="AP53" s="1">
-        <f>AP$51-$AM53+AP$51</f>
+        <f t="shared" ref="AP53:AZ53" si="11">AP$51-$AM53+AP$51</f>
         <v>-1</v>
       </c>
       <c r="AQ53" s="1">
-        <f>AQ$51-$AM53+AQ$51</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="AR53" s="1">
-        <f>AR$51-$AM53+AR$51</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AS53" s="1">
-        <f>AS$51-$AM53+AS$51</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="AT53" s="1">
-        <f>AT$51-$AM53+AT$51</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="AU53" s="1">
-        <f>AU$51-$AM53+AU$51</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AV53" s="1">
-        <f>AV$51-$AM53+AV$51</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="AW53" s="1">
-        <f>AW$51-$AM53+AW$51</f>
+        <f t="shared" si="11"/>
         <v>131</v>
       </c>
       <c r="AX53" s="1">
-        <f>AX$51-$AM53+AX$51</f>
+        <f t="shared" si="11"/>
         <v>131</v>
       </c>
       <c r="AY53" s="1">
-        <f>AY$51-$AM53+AY$51</f>
+        <f t="shared" si="11"/>
         <v>159</v>
       </c>
       <c r="AZ53" s="1">
-        <f>AZ$51-$AM53+AZ$51</f>
+        <f t="shared" si="11"/>
         <v>157</v>
       </c>
     </row>
@@ -2545,43 +2545,43 @@
       </c>
       <c r="AP54" s="11"/>
       <c r="AQ54" s="1">
-        <f>AQ$51-$AM54+AQ$51</f>
+        <f t="shared" ref="AQ54:AZ54" si="12">AQ$51-$AM54+AQ$51</f>
         <v>0</v>
       </c>
       <c r="AR54" s="1">
-        <f>AR$51-$AM54+AR$51</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AS54" s="1">
-        <f>AS$51-$AM54+AS$51</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AT54" s="1">
-        <f>AT$51-$AM54+AT$51</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AU54" s="1">
-        <f>AU$51-$AM54+AU$51</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AV54" s="1">
-        <f>AV$51-$AM54+AV$51</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AW54" s="1">
-        <f>AW$51-$AM54+AW$51</f>
+        <f t="shared" si="12"/>
         <v>132</v>
       </c>
       <c r="AX54" s="1">
-        <f>AX$51-$AM54+AX$51</f>
+        <f t="shared" si="12"/>
         <v>132</v>
       </c>
       <c r="AY54" s="1">
-        <f>AY$51-$AM54+AY$51</f>
+        <f t="shared" si="12"/>
         <v>160</v>
       </c>
       <c r="AZ54" s="1">
-        <f>AZ$51-$AM54+AZ$51</f>
+        <f t="shared" si="12"/>
         <v>158</v>
       </c>
     </row>
@@ -2642,39 +2642,39 @@
       </c>
       <c r="AQ55" s="11"/>
       <c r="AR55" s="1">
-        <f>AR$51-$AM55+AR$51</f>
+        <f t="shared" ref="AR55:AZ55" si="13">AR$51-$AM55+AR$51</f>
         <v>2</v>
       </c>
       <c r="AS55" s="1">
-        <f>AS$51-$AM55+AS$51</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AT55" s="1">
-        <f>AT$51-$AM55+AT$51</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AU55" s="1">
-        <f>AU$51-$AM55+AU$51</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="AV55" s="1">
-        <f>AV$51-$AM55+AV$51</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AW55" s="1">
-        <f>AW$51-$AM55+AW$51</f>
+        <f t="shared" si="13"/>
         <v>132</v>
       </c>
       <c r="AX55" s="1">
-        <f>AX$51-$AM55+AX$51</f>
+        <f t="shared" si="13"/>
         <v>132</v>
       </c>
       <c r="AY55" s="1">
-        <f>AY$51-$AM55+AY$51</f>
+        <f t="shared" si="13"/>
         <v>160</v>
       </c>
       <c r="AZ55" s="1">
-        <f>AZ$51-$AM55+AZ$51</f>
+        <f t="shared" si="13"/>
         <v>158</v>
       </c>
     </row>
@@ -2723,35 +2723,35 @@
       </c>
       <c r="AR56" s="11"/>
       <c r="AS56" s="1">
-        <f>AS$51-$AM56+AS$51</f>
+        <f t="shared" ref="AS56:AZ56" si="14">AS$51-$AM56+AS$51</f>
         <v>-1</v>
       </c>
       <c r="AT56" s="1">
-        <f>AT$51-$AM56+AT$51</f>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="AU56" s="1">
-        <f>AU$51-$AM56+AU$51</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AV56" s="1">
-        <f>AV$51-$AM56+AV$51</f>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="AW56" s="1">
-        <f>AW$51-$AM56+AW$51</f>
+        <f t="shared" si="14"/>
         <v>131</v>
       </c>
       <c r="AX56" s="1">
-        <f>AX$51-$AM56+AX$51</f>
+        <f t="shared" si="14"/>
         <v>131</v>
       </c>
       <c r="AY56" s="1">
-        <f>AY$51-$AM56+AY$51</f>
+        <f t="shared" si="14"/>
         <v>159</v>
       </c>
       <c r="AZ56" s="1">
-        <f>AZ$51-$AM56+AZ$51</f>
+        <f t="shared" si="14"/>
         <v>157</v>
       </c>
     </row>
@@ -2783,6 +2783,9 @@
       <c r="AB57" s="1">
         <v>4</v>
       </c>
+      <c r="AF57" s="1">
+        <v>89</v>
+      </c>
       <c r="AL57" s="1">
         <v>5</v>
       </c>
@@ -2791,31 +2794,31 @@
       </c>
       <c r="AS57" s="11"/>
       <c r="AT57" s="1">
-        <f>AT$51-$AM57+AT$51</f>
+        <f t="shared" ref="AT57:AZ57" si="15">AT$51-$AM57+AT$51</f>
         <v>0</v>
       </c>
       <c r="AU57" s="1">
-        <f>AU$51-$AM57+AU$51</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="AV57" s="1">
-        <f>AV$51-$AM57+AV$51</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AW57" s="1">
-        <f>AW$51-$AM57+AW$51</f>
+        <f t="shared" si="15"/>
         <v>132</v>
       </c>
       <c r="AX57" s="1">
-        <f>AX$51-$AM57+AX$51</f>
+        <f t="shared" si="15"/>
         <v>132</v>
       </c>
       <c r="AY57" s="1">
-        <f>AY$51-$AM57+AY$51</f>
+        <f t="shared" si="15"/>
         <v>160</v>
       </c>
       <c r="AZ57" s="1">
-        <f>AZ$51-$AM57+AZ$51</f>
+        <f t="shared" si="15"/>
         <v>158</v>
       </c>
     </row>
@@ -2849,27 +2852,27 @@
       </c>
       <c r="AT58" s="11"/>
       <c r="AU58" s="1">
-        <f>AU$51-$AM58+AU$51</f>
+        <f t="shared" ref="AU58:AZ58" si="16">AU$51-$AM58+AU$51</f>
         <v>2</v>
       </c>
       <c r="AV58" s="1">
-        <f>AV$51-$AM58+AV$51</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AW58" s="1">
-        <f>AW$51-$AM58+AW$51</f>
+        <f t="shared" si="16"/>
         <v>132</v>
       </c>
       <c r="AX58" s="1">
-        <f>AX$51-$AM58+AX$51</f>
+        <f t="shared" si="16"/>
         <v>132</v>
       </c>
       <c r="AY58" s="1">
-        <f>AY$51-$AM58+AY$51</f>
+        <f t="shared" si="16"/>
         <v>160</v>
       </c>
       <c r="AZ58" s="1">
-        <f>AZ$51-$AM58+AZ$51</f>
+        <f t="shared" si="16"/>
         <v>158</v>
       </c>
     </row>

</xml_diff>